<commit_message>
Matrix figure: added colors to areas.
</commit_message>
<xml_diff>
--- a/Connect_ProjProj.xlsx
+++ b/Connect_ProjProj.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="15160" yWindow="40" windowWidth="11680" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1 - Table 1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -97,6 +97,38 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF008000"/>
+      <name val="System Font Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF0000FF"/>
+      <name val="System Font Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFD8AE04"/>
+      <name val="System Font Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="System Font Regular"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -191,15 +223,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -209,8 +252,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,9 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -672,214 +721,214 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="34" customHeight="1">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="34" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="34" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="34" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="6"/>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" ht="34" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="34" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="7"/>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="34" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="6"/>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="9" max="16383" man="1"/>
@@ -889,7 +938,7 @@
   </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>